<commit_message>
Updated login data xlsx
</commit_message>
<xml_diff>
--- a/testData/loginData.xlsx
+++ b/testData/loginData.xlsx
@@ -365,12 +365,12 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -394,7 +394,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>